<commit_message>
pending updates mostly mcu schematic
</commit_message>
<xml_diff>
--- a/Documentation/BuckThermal.xlsx
+++ b/Documentation/BuckThermal.xlsx
@@ -45,6 +45,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="D2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>kipman725:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ALLPCB minimum</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>kipman725:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+size of thermal 'coin' from pcb</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E4" authorId="0">
       <text>
         <r>
@@ -75,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>R_jc</t>
   </si>
@@ -92,9 +140,6 @@
     <t>PCB thickness</t>
   </si>
   <si>
-    <t>Coper weight [Oz]</t>
-  </si>
-  <si>
     <t>Lambda_Cu</t>
   </si>
   <si>
@@ -119,7 +164,37 @@
     <t>W/mK</t>
   </si>
   <si>
-    <t>Rth</t>
+    <t>Pad is Hi-flow 300p</t>
+  </si>
+  <si>
+    <t>Rth pad</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Solder</t>
+  </si>
+  <si>
+    <t>Assumed included in device Rth</t>
+  </si>
+  <si>
+    <t>PCB top copper</t>
+  </si>
+  <si>
+    <t>Via</t>
+  </si>
+  <si>
+    <t>PCB bottom copper</t>
+  </si>
+  <si>
+    <t>Shim w/mk</t>
+  </si>
+  <si>
+    <t>Shim thickness</t>
+  </si>
+  <si>
+    <t>Rth Shim</t>
   </si>
 </sst>
 </file>
@@ -189,10 +264,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,14 +572,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" customWidth="1"/>
@@ -510,16 +589,14 @@
     <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C1" s="2"/>
       <c r="D1" t="s">
         <v>2</v>
       </c>
@@ -530,28 +607,27 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
+      <c r="M1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.4</v>
       </c>
       <c r="B2">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <f>C2*0.000035</f>
-        <v>6.9999999999999994E-5</v>
+        <v>34</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.8034E-5</v>
       </c>
       <c r="E2" s="1">
         <v>2.9999999999999997E-4</v>
@@ -564,53 +640,97 @@
       </c>
       <c r="H2" s="1">
         <f>1/G2*F2/(PI()*((E2/2)^2-(E2/2-D2)^2))</f>
-        <v>49.427000960215956</v>
+        <v>156.49531017807277</v>
       </c>
       <c r="I2" s="1">
         <f>H2/B2</f>
-        <v>2.7459444977897753</v>
+        <v>4.6028032405315518</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="M4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>6.4999999999999997E-3</v>
       </c>
       <c r="B5" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>6.1999999999999998E-3</v>
       </c>
       <c r="C5" s="1">
         <f>A5*B5</f>
-        <v>3.0000000000000001E-5</v>
+        <v>4.0299999999999997E-5</v>
       </c>
       <c r="D5" s="1">
-        <v>5.0000000000000001E-4</v>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="E5" s="1">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="F5" s="1">
         <f>D5/(C5*E5)</f>
-        <v>13.888888888888889</v>
+        <v>0.38771712158808941</v>
+      </c>
+      <c r="M5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>205</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C8" s="1">
+        <f>B8/(A8*C5)</f>
+        <v>0.6052169702838468</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="M8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>